<commit_message>
add billcounter to transaction page& excel. add modal for transaction page
</commit_message>
<xml_diff>
--- a/wwwroot/RegulatorExcel/InputTemplate/Transaction.xlsx
+++ b/wwwroot/RegulatorExcel/InputTemplate/Transaction.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27321"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\Git\EJLogViewer\EJLogViewer\Reports\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F407E5C1-D1D0-429D-B4B9-A4DE3992F866}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="3570" windowWidth="20730" windowHeight="11385"/>
+    <workbookView xWindow="1560" yWindow="3570" windowWidth="20730" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,6 +26,9 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,7 +36,43 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+  <si>
+    <t>ธนาคาร :</t>
+  </si>
+  <si>
+    <t>GHB Bank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ข้อมูลวันที่ : </t>
+  </si>
+  <si>
+    <t>เรียงข้อมูลด้วย :</t>
+  </si>
+  <si>
+    <t>เรียงจาก :</t>
+  </si>
+  <si>
+    <t xml:space="preserve">หมายเลขตู้ : </t>
+  </si>
+  <si>
+    <t>ชื่อสาขา :</t>
+  </si>
+  <si>
+    <t>Status :</t>
+  </si>
+  <si>
+    <t xml:space="preserve">จำนวน : </t>
+  </si>
+  <si>
+    <t>รายการ</t>
+  </si>
+  <si>
+    <t>Transaction Type :</t>
+  </si>
+  <si>
+    <t>Response code :</t>
+  </si>
   <si>
     <t>No.</t>
   </si>
@@ -67,70 +107,22 @@
     <t>Amount</t>
   </si>
   <si>
+    <t>Fee</t>
+  </si>
+  <si>
     <t>Retract Amount</t>
   </si>
   <si>
+    <t>Bill Counter</t>
+  </si>
+  <si>
     <t>RC</t>
-  </si>
-  <si>
-    <t>Fee</t>
-  </si>
-  <si>
-    <t>Branch</t>
-  </si>
-  <si>
-    <t>2020-06-01 00:00:00 ถึง 2020-06-02 23:59:59</t>
-  </si>
-  <si>
-    <t>AAAA</t>
-  </si>
-  <si>
-    <t>เรียงข้อมูลด้วย :</t>
-  </si>
-  <si>
-    <t>Transaction Type :</t>
-  </si>
-  <si>
-    <t>เรียงจาก :</t>
-  </si>
-  <si>
-    <t>Status :</t>
-  </si>
-  <si>
-    <t>Response code :</t>
-  </si>
-  <si>
-    <t>เลือกทั้งหมด</t>
-  </si>
-  <si>
-    <t>น้อยไปมาก</t>
-  </si>
-  <si>
-    <t>Date Time</t>
-  </si>
-  <si>
-    <t>รายการ</t>
-  </si>
-  <si>
-    <t>ชื่อสาขา :</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ข้อมูลวันที่ : </t>
-  </si>
-  <si>
-    <t xml:space="preserve">หมายเลขตู้ : </t>
-  </si>
-  <si>
-    <t xml:space="preserve">จำนวน : </t>
-  </si>
-  <si>
-    <t>ธนาคาร :</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="187" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
@@ -294,7 +286,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -312,13 +304,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="187" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="187" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -330,19 +322,16 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="187" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="187" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -351,15 +340,24 @@
     <xf numFmtId="187" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="187" fontId="5" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -369,26 +367,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="187" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="187" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="187" fontId="5" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -423,13 +412,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>246731</xdr:colOff>
+      <xdr:colOff>238125</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>103283</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -757,32 +752,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="166" zoomScaleNormal="166" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="11.25"/>
   <cols>
-    <col min="1" max="2" width="5.875" style="13" customWidth="1"/>
-    <col min="3" max="3" width="15.375" style="15" customWidth="1"/>
-    <col min="4" max="4" width="7.625" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.375" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.625" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.375" style="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.375" style="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.375" style="16" customWidth="1"/>
-    <col min="10" max="10" width="5.375" style="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.125" style="13" customWidth="1"/>
-    <col min="12" max="12" width="5.75" style="13" customWidth="1"/>
-    <col min="13" max="13" width="11.875" style="13" customWidth="1"/>
-    <col min="14" max="14" width="6.25" style="13" customWidth="1"/>
-    <col min="15" max="16384" width="9.125" style="6"/>
+    <col min="1" max="2" width="5.875" style="9" customWidth="1"/>
+    <col min="3" max="3" width="15.375" style="14" customWidth="1"/>
+    <col min="4" max="4" width="10" style="9" customWidth="1"/>
+    <col min="5" max="5" width="8.375" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.625" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.375" style="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.375" style="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.375" style="15" customWidth="1"/>
+    <col min="10" max="10" width="5.375" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.125" style="9" customWidth="1"/>
+    <col min="12" max="12" width="5.75" style="9" customWidth="1"/>
+    <col min="13" max="14" width="11.875" style="9" customWidth="1"/>
+    <col min="15" max="15" width="6.25" style="9" customWidth="1"/>
+    <col min="16" max="16" width="9.125" style="6" customWidth="1"/>
+    <col min="17" max="16384" width="9.125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="18.75" customHeight="1">
+    <row r="1" spans="1:15" ht="18.75" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -796,168 +792,154 @@
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
-      <c r="N1" s="5"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="5"/>
     </row>
-    <row r="2" spans="1:14" ht="18.75" customHeight="1">
-      <c r="A2" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="28"/>
+    <row r="2" spans="1:15" ht="18.75" customHeight="1">
+      <c r="A2" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="30"/>
     </row>
-    <row r="3" spans="1:14" ht="18.75" customHeight="1">
-      <c r="A3" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
+    <row r="3" spans="1:15" ht="18.75" customHeight="1">
+      <c r="A3" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="28"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
       <c r="G3" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="20" t="s">
-        <v>24</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="H3" s="19"/>
       <c r="I3" s="8"/>
       <c r="J3" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="K3" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="10"/>
+        <v>4</v>
+      </c>
+      <c r="K3" s="20"/>
+      <c r="O3" s="10"/>
     </row>
-    <row r="4" spans="1:14" ht="18.75" customHeight="1">
-      <c r="A4" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="29"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
+    <row r="4" spans="1:15" ht="18.75" customHeight="1">
+      <c r="A4" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="28"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
       <c r="G4" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H4" s="20" t="s">
-        <v>22</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="H4" s="19"/>
       <c r="I4" s="8"/>
       <c r="J4" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K4" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="10"/>
+        <v>7</v>
+      </c>
+      <c r="K4" s="20"/>
+      <c r="O4" s="10"/>
     </row>
-    <row r="5" spans="1:14" ht="18.75" customHeight="1">
-      <c r="A5" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="24"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="18" t="s">
-        <v>25</v>
+    <row r="5" spans="1:15" ht="18.75" customHeight="1">
+      <c r="A5" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="26"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="17" t="s">
+        <v>9</v>
       </c>
       <c r="E5" s="11"/>
       <c r="F5" s="11"/>
       <c r="G5" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" s="20" t="s">
-        <v>22</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="H5" s="19"/>
       <c r="I5" s="12"/>
       <c r="J5" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="K5" s="22" t="s">
-        <v>22</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="K5" s="21"/>
       <c r="L5" s="11"/>
       <c r="M5" s="11"/>
-      <c r="N5" s="14"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="13"/>
     </row>
-    <row r="6" spans="1:14" ht="18.75" customHeight="1">
-      <c r="A6" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="31" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="30" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6" s="30" t="s">
-        <v>5</v>
-      </c>
-      <c r="G6" s="32" t="s">
-        <v>6</v>
-      </c>
-      <c r="H6" s="32" t="s">
-        <v>7</v>
-      </c>
-      <c r="I6" s="32" t="s">
-        <v>8</v>
-      </c>
-      <c r="J6" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="K6" s="30" t="s">
-        <v>10</v>
-      </c>
-      <c r="L6" s="30" t="s">
+    <row r="6" spans="1:15" ht="18.75" customHeight="1">
+      <c r="A6" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="M6" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="N6" s="30" t="s">
-        <v>12</v>
+      <c r="C6" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="K6" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="L6" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="M6" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="N6" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="O6" s="22" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A2:G2"/>
-    <mergeCell ref="H2:N2"/>
+    <mergeCell ref="H2:O2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C3:F3"/>
     <mergeCell ref="C4:D4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="landscape"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>